<commit_message>
Update conferencia produtos zerados === produtos perdidos.
</commit_message>
<xml_diff>
--- a/app/static/uploads/tabela_planilha.xlsx
+++ b/app/static/uploads/tabela_planilha.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37583E98-D8EF-4058-8F09-2D5960563769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBFCBF7E-2C0C-4F32-9D05-A35688C1E719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1EFC1A00-DCA6-4636-A2BD-065FF7E4312E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="9">
   <si>
     <t>CODIGO</t>
   </si>
@@ -47,14 +47,29 @@
     <t>FISICO</t>
   </si>
   <si>
-    <t>DIFERENCA</t>
+    <t>LOJAS</t>
+  </si>
+  <si>
+    <t>AJUSTE</t>
+  </si>
+  <si>
+    <t>DIVERGENCIA</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Não </t>
+  </si>
+  <si>
+    <t>Não</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,14 +79,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -127,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,9 +147,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -459,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C256A14-3F27-49E5-A34A-F88D72D47B2A}">
-  <dimension ref="A1:D211"/>
+  <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:B208"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F52" sqref="A52:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,9 +474,10 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -485,8 +490,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>65</v>
       </c>
@@ -496,12 +507,17 @@
       <c r="C2" s="1">
         <v>59</v>
       </c>
-      <c r="D2" s="1">
-        <f>-B2+C2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2365</v>
       </c>
@@ -511,12 +527,17 @@
       <c r="C3" s="1">
         <v>8</v>
       </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D60" si="0">-B3+C3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2355</v>
       </c>
@@ -526,12 +547,17 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>2364</v>
       </c>
@@ -541,12 +567,17 @@
       <c r="C5" s="1">
         <v>489</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5429</v>
       </c>
@@ -556,12 +587,17 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>-16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>12</v>
       </c>
@@ -571,12 +607,17 @@
       <c r="C7" s="1">
         <v>298</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>3794</v>
       </c>
@@ -586,12 +627,17 @@
       <c r="C8" s="1">
         <v>428</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>10286</v>
       </c>
@@ -601,12 +647,17 @@
       <c r="C9" s="1">
         <v>42</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>-33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8883</v>
       </c>
@@ -616,12 +667,17 @@
       <c r="C10" s="1">
         <v>2144</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>339</v>
       </c>
@@ -631,12 +687,17 @@
       <c r="C11" s="1">
         <v>240</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>1795</v>
       </c>
@@ -646,12 +707,17 @@
       <c r="C12" s="1">
         <v>10</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>5517</v>
       </c>
@@ -661,12 +727,17 @@
       <c r="C13" s="1">
         <v>40</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>5415</v>
       </c>
@@ -676,12 +747,17 @@
       <c r="C14" s="1">
         <v>1354</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="D14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>5518</v>
       </c>
@@ -691,12 +767,17 @@
       <c r="C15" s="1">
         <v>133</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>4191</v>
       </c>
@@ -706,12 +787,17 @@
       <c r="C16" s="1">
         <v>783</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="D16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>3792</v>
       </c>
@@ -721,12 +807,17 @@
       <c r="C17" s="1">
         <v>104</v>
       </c>
-      <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>1796</v>
       </c>
@@ -736,12 +827,17 @@
       <c r="C18" s="1">
         <v>10</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>368</v>
       </c>
@@ -751,12 +847,17 @@
       <c r="C19" s="1">
         <v>296</v>
       </c>
-      <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>11128</v>
       </c>
@@ -766,12 +867,17 @@
       <c r="C20" s="1">
         <v>38</v>
       </c>
-      <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>33</v>
       </c>
@@ -781,12 +887,17 @@
       <c r="C21" s="1">
         <v>175</v>
       </c>
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>7796</v>
       </c>
@@ -796,12 +907,17 @@
       <c r="C22" s="1">
         <v>0</v>
       </c>
-      <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>7729</v>
       </c>
@@ -811,12 +927,17 @@
       <c r="C23" s="1">
         <v>54</v>
       </c>
-      <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>11123</v>
       </c>
@@ -826,12 +947,17 @@
       <c r="C24" s="1">
         <v>11</v>
       </c>
-      <c r="D24" s="1">
-        <f t="shared" si="0"/>
-        <v>-6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>8880</v>
       </c>
@@ -841,12 +967,17 @@
       <c r="C25" s="1">
         <v>1</v>
       </c>
-      <c r="D25" s="1">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="D25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>1466</v>
       </c>
@@ -856,12 +987,17 @@
       <c r="C26" s="1">
         <v>0</v>
       </c>
-      <c r="D26" s="1">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="D26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>3</v>
       </c>
@@ -871,12 +1007,17 @@
       <c r="C27" s="1">
         <v>55</v>
       </c>
-      <c r="D27" s="1">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="D27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>2814</v>
       </c>
@@ -886,12 +1027,17 @@
       <c r="C28" s="1">
         <v>254</v>
       </c>
-      <c r="D28" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="D28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>2813</v>
       </c>
@@ -901,12 +1047,17 @@
       <c r="C29" s="1">
         <v>33</v>
       </c>
-      <c r="D29" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>1468</v>
       </c>
@@ -916,12 +1067,17 @@
       <c r="C30" s="1">
         <v>31</v>
       </c>
-      <c r="D30" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>7263</v>
       </c>
@@ -931,12 +1087,17 @@
       <c r="C31" s="1">
         <v>12</v>
       </c>
-      <c r="D31" s="1">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="D31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>11252</v>
       </c>
@@ -946,12 +1107,17 @@
       <c r="C32" s="1">
         <v>0</v>
       </c>
-      <c r="D32" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="D32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>10296</v>
       </c>
@@ -961,12 +1127,17 @@
       <c r="C33" s="1">
         <v>3</v>
       </c>
-      <c r="D33" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="D33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>10654</v>
       </c>
@@ -976,12 +1147,17 @@
       <c r="C34" s="1">
         <v>30</v>
       </c>
-      <c r="D34" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="D34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>10782</v>
       </c>
@@ -991,12 +1167,17 @@
       <c r="C35" s="1">
         <v>0</v>
       </c>
-      <c r="D35" s="1">
-        <f t="shared" si="0"/>
-        <v>-103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="D35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>11126</v>
       </c>
@@ -1006,12 +1187,17 @@
       <c r="C36" s="1">
         <v>213</v>
       </c>
-      <c r="D36" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="D36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>405</v>
       </c>
@@ -1021,12 +1207,17 @@
       <c r="C37" s="1">
         <v>25</v>
       </c>
-      <c r="D37" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="D37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>10746</v>
       </c>
@@ -1036,12 +1227,17 @@
       <c r="C38" s="1">
         <v>20</v>
       </c>
-      <c r="D38" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="D38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>11314</v>
       </c>
@@ -1051,12 +1247,17 @@
       <c r="C39" s="1">
         <v>826</v>
       </c>
-      <c r="D39" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="D39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>9074</v>
       </c>
@@ -1066,12 +1267,17 @@
       <c r="C40" s="1">
         <v>373</v>
       </c>
-      <c r="D40" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="D40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>10067</v>
       </c>
@@ -1081,12 +1287,17 @@
       <c r="C41" s="1">
         <v>0</v>
       </c>
-      <c r="D41" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="D41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>11340</v>
       </c>
@@ -1096,12 +1307,17 @@
       <c r="C42" s="1">
         <v>57</v>
       </c>
-      <c r="D42" s="1">
-        <f>-B42+C42</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="D42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="1">
         <v>11341</v>
       </c>
@@ -1111,12 +1327,17 @@
       <c r="C43" s="1">
         <v>27</v>
       </c>
-      <c r="D43" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="D43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1">
         <v>10747</v>
       </c>
@@ -1126,12 +1347,17 @@
       <c r="C44" s="1">
         <v>6</v>
       </c>
-      <c r="D44" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="D44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1">
         <v>6</v>
       </c>
@@ -1141,12 +1367,17 @@
       <c r="C45" s="1">
         <v>474</v>
       </c>
-      <c r="D45" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="D45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1">
         <v>3144</v>
       </c>
@@ -1156,12 +1387,17 @@
       <c r="C46" s="1">
         <v>0</v>
       </c>
-      <c r="D46" s="1">
-        <f t="shared" si="0"/>
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="D46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="1">
         <v>6582</v>
       </c>
@@ -1171,12 +1407,17 @@
       <c r="C47" s="1">
         <v>90</v>
       </c>
-      <c r="D47" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="D47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="1">
         <v>8870</v>
       </c>
@@ -1186,12 +1427,17 @@
       <c r="C48" s="1">
         <v>475</v>
       </c>
-      <c r="D48" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="D48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="1">
         <v>11313</v>
       </c>
@@ -1201,12 +1447,17 @@
       <c r="C49" s="1">
         <v>168</v>
       </c>
-      <c r="D49" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="D49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="1">
         <v>4282</v>
       </c>
@@ -1216,12 +1467,17 @@
       <c r="C50" s="1">
         <v>0</v>
       </c>
-      <c r="D50" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="D50" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="1">
         <v>242</v>
       </c>
@@ -1231,93 +1487,89 @@
       <c r="C51" s="1">
         <v>5304</v>
       </c>
-      <c r="D51" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="5">
-        <v>11317</v>
-      </c>
-      <c r="B52" s="5">
-        <v>7</v>
-      </c>
-      <c r="C52" s="5">
-        <v>7</v>
-      </c>
-      <c r="D52" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="D51" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:6">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:6">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:6">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:6">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:6">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:6">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:6">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:6">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:6">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:6">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:6">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>

</xml_diff>